<commit_message>
add paylaod for dataElement/ optionSet/ options post method
</commit_message>
<xml_diff>
--- a/Excel to json convertor/sample-format/NIPI Atru Data_event_coordinate_import.xlsx
+++ b/Excel to json convertor/sample-format/NIPI Atru Data_event_coordinate_import.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mithilesh Thakur\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0C5ECC-84BA-4749-A88F-655740199C6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108632F2-308A-4658-A7F8-5C990885BAE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8E413B3D-A7A0-4B71-B238-4275582DC323}"/>
   </bookViews>

</xml_diff>

<commit_message>
update payload for datavalue delete
</commit_message>
<xml_diff>
--- a/Excel to json convertor/sample-format/NIPI Atru Data_event_coordinate_import.xlsx
+++ b/Excel to json convertor/sample-format/NIPI Atru Data_event_coordinate_import.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mithilesh Thakur\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108632F2-308A-4658-A7F8-5C990885BAE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0C5ECC-84BA-4749-A88F-655740199C6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8E413B3D-A7A0-4B71-B238-4275582DC323}"/>
   </bookViews>

</xml_diff>